<commit_message>
add svm, knn, and naivebayes algorithms
</commit_message>
<xml_diff>
--- a/Results/merged_comparison_results.xlsx
+++ b/Results/merged_comparison_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Semester 3\Applied Machine Learning\Practice2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Semester 3\Applied Machine Learning\Practice2\ML-Project-Breast-Cancer\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF010DB-6C4B-4A2F-8F7A-42EB644625C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A359CEEB-A7B1-4915-8C01-CE0A28A9F0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="18195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -518,12 +518,12 @@
   <dimension ref="A1:R97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97:F97"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="93" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="95.265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.53125" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="11.73046875" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>